<commit_message>
assignment marking guide check
</commit_message>
<xml_diff>
--- a/GlassCat_AS2_Moment/App_Data/FIT5192-A2-MarkingSheet.xlsx
+++ b/GlassCat_AS2_Moment/App_Data/FIT5192-A2-MarkingSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Seu_Monash_2019_Spring\Murray_FIT5192\AS2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\VS\GlassCat_AS2_Moment\GlassCat_AS2_Moment\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -826,7 +826,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1004,63 +1004,63 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1118,13 +1118,22 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1348,14 +1357,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1713,52 +1722,52 @@
       <c r="A5" s="9"/>
     </row>
     <row r="6" spans="1:7" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="68"/>
+      <c r="B6" s="77"/>
     </row>
     <row r="7" spans="1:7" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
     </row>
     <row r="8" spans="1:7" s="9" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -1767,45 +1776,45 @@
       <c r="A12" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
     </row>
     <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="80"/>
-      <c r="D14" s="81"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="72"/>
     </row>
     <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="74" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
     </row>
     <row r="17" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1816,124 +1825,124 @@
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="75"/>
     </row>
     <row r="20" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="74"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
     </row>
     <row r="22" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="71" t="s">
+      <c r="A22" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
     </row>
     <row r="24" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="70" t="s">
+      <c r="A24" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
     </row>
     <row r="25" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="70" t="s">
+      <c r="A25" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
     </row>
     <row r="26" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="70" t="s">
+      <c r="A26" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="71"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="71"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
     </row>
     <row r="27" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="70" t="s">
+      <c r="A27" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="71"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="71"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
     </row>
     <row r="28" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="70" t="s">
+      <c r="A28" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="71"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
     </row>
     <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="71" t="s">
+      <c r="A29" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
     </row>
     <row r="30" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="71" t="s">
+      <c r="A30" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
     </row>
     <row r="31" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="71" t="s">
+      <c r="A31" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="71"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71"/>
+      <c r="B31" s="69"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
     </row>
     <row r="32" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="70" t="s">
+      <c r="A32" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="71"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="71"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
     </row>
     <row r="33" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="70" t="s">
+      <c r="A33" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="71"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
@@ -1944,12 +1953,12 @@
       <c r="D34" s="11"/>
     </row>
     <row r="35" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="69" t="s">
+      <c r="A35" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="69"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="69"/>
+      <c r="B35" s="78"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="78"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
@@ -1959,17 +1968,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="A28:D28"/>
@@ -1986,6 +1984,17 @@
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A24:D24"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.36" bottom="0.39" header="0.34" footer="0.37"/>
@@ -2001,8 +2010,8 @@
   </sheetPr>
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2071,18 +2080,18 @@
         <f>'Assessment cover sheet'!A12</f>
         <v>Student one full name &amp; Student ID:</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="str">
         <f>'Assessment cover sheet'!A13</f>
         <v>Student two full name &amp; Student ID:</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="49" t="str">
@@ -2124,14 +2133,14 @@
       <c r="A14" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="63"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="16"/>
     </row>
     <row r="15" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="102">
+      <c r="B15" s="106">
         <v>2</v>
       </c>
       <c r="C15" s="16"/>
@@ -2140,7 +2149,7 @@
       <c r="A16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="103">
         <v>1</v>
       </c>
       <c r="C16" s="16"/>
@@ -2149,7 +2158,7 @@
       <c r="A17" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="103">
         <v>1</v>
       </c>
       <c r="C17" s="16"/>
@@ -2159,7 +2168,7 @@
       <c r="A18" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="102">
+      <c r="B18" s="66">
         <v>2</v>
       </c>
       <c r="C18" s="16"/>
@@ -2168,7 +2177,7 @@
       <c r="A19" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="103">
         <v>2</v>
       </c>
       <c r="C19" s="16"/>
@@ -2177,28 +2186,28 @@
       <c r="A20" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="102">
+      <c r="B20" s="66">
         <v>1</v>
       </c>
       <c r="C20" s="16"/>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
-      <c r="B21" s="16"/>
+      <c r="B21" s="103"/>
       <c r="C21" s="16"/>
     </row>
     <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="63"/>
+      <c r="B22" s="102"/>
       <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="102">
+      <c r="B23" s="66">
         <v>2</v>
       </c>
       <c r="C23" s="16"/>
@@ -2207,7 +2216,7 @@
       <c r="A24" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="102">
+      <c r="B24" s="66">
         <v>1</v>
       </c>
       <c r="C24" s="16"/>
@@ -2216,28 +2225,28 @@
       <c r="A25" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="65">
         <v>2</v>
       </c>
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
-      <c r="B26" s="7"/>
+      <c r="B26" s="101"/>
       <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="64"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="101">
+      <c r="B28" s="65">
         <v>5</v>
       </c>
       <c r="C28" s="7"/>
@@ -2246,7 +2255,7 @@
       <c r="A29" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="101">
+      <c r="B29" s="65">
         <v>5</v>
       </c>
       <c r="C29" s="7"/>
@@ -2255,7 +2264,7 @@
       <c r="A30" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="101">
+      <c r="B30" s="65">
         <v>1</v>
       </c>
       <c r="C30" s="7"/>
@@ -2264,7 +2273,7 @@
       <c r="A31" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="101">
+      <c r="B31" s="65">
         <v>1</v>
       </c>
       <c r="C31" s="7"/>
@@ -2273,28 +2282,28 @@
       <c r="A32" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="101">
+      <c r="B32" s="65">
         <v>1</v>
       </c>
       <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
-      <c r="B33" s="7"/>
+      <c r="B33" s="101"/>
       <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="64"/>
+      <c r="B34" s="104"/>
       <c r="C34" s="7"/>
     </row>
     <row r="35" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="101">
+      <c r="B35" s="65">
         <v>3</v>
       </c>
       <c r="C35" s="7"/>
@@ -2303,7 +2312,7 @@
       <c r="A36" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="65">
         <v>2</v>
       </c>
       <c r="C36" s="7"/>
@@ -2312,7 +2321,7 @@
       <c r="A37" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="65">
         <v>2</v>
       </c>
       <c r="C37" s="7"/>
@@ -2321,28 +2330,28 @@
       <c r="A38" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="65">
         <v>1</v>
       </c>
       <c r="C38" s="7"/>
     </row>
     <row r="39" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
-      <c r="B39" s="7"/>
+      <c r="B39" s="101"/>
       <c r="C39" s="7"/>
     </row>
     <row r="40" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="65"/>
+      <c r="B40" s="105"/>
       <c r="C40" s="38"/>
     </row>
     <row r="41" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="103">
+      <c r="B41" s="67">
         <v>1</v>
       </c>
       <c r="C41" s="38"/>
@@ -2351,7 +2360,7 @@
       <c r="A42" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="103">
+      <c r="B42" s="67">
         <v>1</v>
       </c>
       <c r="C42" s="38"/>
@@ -2360,7 +2369,7 @@
       <c r="A43" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="103">
+      <c r="B43" s="67">
         <v>1</v>
       </c>
       <c r="C43" s="38"/>
@@ -2369,28 +2378,28 @@
       <c r="A44" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="65">
         <v>1</v>
       </c>
       <c r="C44" s="7"/>
     </row>
     <row r="45" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
-      <c r="B45" s="7"/>
+      <c r="B45" s="101"/>
       <c r="C45" s="7"/>
     </row>
     <row r="46" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B46" s="64"/>
+      <c r="B46" s="104"/>
       <c r="C46" s="7"/>
     </row>
     <row r="47" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="101">
+      <c r="B47" s="65">
         <v>2</v>
       </c>
       <c r="C47" s="7"/>
@@ -2399,28 +2408,28 @@
       <c r="A48" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="65">
         <v>1</v>
       </c>
       <c r="C48" s="7"/>
     </row>
     <row r="49" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17"/>
-      <c r="B49" s="7"/>
+      <c r="B49" s="101"/>
       <c r="C49" s="7"/>
     </row>
     <row r="50" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B50" s="64"/>
+      <c r="B50" s="104"/>
       <c r="C50" s="7"/>
     </row>
     <row r="51" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="101">
         <v>5</v>
       </c>
       <c r="C51" s="7"/>
@@ -2429,28 +2438,28 @@
       <c r="A52" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="101">
         <v>1</v>
       </c>
       <c r="C52" s="7"/>
     </row>
     <row r="53" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17"/>
-      <c r="B53" s="7"/>
+      <c r="B53" s="101"/>
       <c r="C53" s="7"/>
     </row>
     <row r="54" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="64"/>
+      <c r="B54" s="104"/>
       <c r="C54" s="7"/>
     </row>
     <row r="55" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="65">
         <v>5</v>
       </c>
       <c r="C55" s="7"/>
@@ -2459,35 +2468,35 @@
       <c r="A56" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B56" s="65">
         <v>1</v>
       </c>
       <c r="C56" s="7"/>
     </row>
     <row r="57" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
-      <c r="B57" s="7"/>
+      <c r="B57" s="101"/>
       <c r="C57" s="7"/>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B58" s="7"/>
+      <c r="B58" s="101"/>
       <c r="C58" s="7"/>
     </row>
     <row r="59" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="B59" s="64"/>
+      <c r="B59" s="104"/>
       <c r="C59" s="7"/>
     </row>
     <row r="60" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="101">
         <v>1</v>
       </c>
       <c r="C60" s="7"/>
@@ -2496,7 +2505,7 @@
       <c r="A61" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B61" s="101">
         <v>2</v>
       </c>
       <c r="C61" s="7"/>
@@ -2505,7 +2514,7 @@
       <c r="A62" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B62" s="7">
+      <c r="B62" s="101">
         <v>1</v>
       </c>
       <c r="C62" s="7"/>
@@ -2514,28 +2523,28 @@
       <c r="A63" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B63" s="7">
+      <c r="B63" s="101">
         <v>1</v>
       </c>
       <c r="C63" s="7"/>
     </row>
     <row r="64" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="53"/>
-      <c r="B64" s="7"/>
+      <c r="B64" s="101"/>
       <c r="C64" s="7"/>
     </row>
     <row r="65" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="B65" s="64"/>
+      <c r="B65" s="104"/>
       <c r="C65" s="7"/>
     </row>
     <row r="66" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="B66" s="7">
+      <c r="B66" s="101">
         <v>2</v>
       </c>
       <c r="C66" s="7"/>
@@ -2544,7 +2553,7 @@
       <c r="A67" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="B67" s="7">
+      <c r="B67" s="101">
         <v>1</v>
       </c>
       <c r="C67" s="7"/>
@@ -2553,7 +2562,7 @@
       <c r="A68" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="7">
+      <c r="B68" s="101">
         <v>1</v>
       </c>
       <c r="C68" s="7"/>
@@ -2562,35 +2571,42 @@
       <c r="A69" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69" s="101">
         <v>1</v>
       </c>
       <c r="C69" s="7"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="101"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B71" s="101">
         <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="35"/>
+      <c r="B72" s="101"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="B73" s="7">
+      <c r="B73" s="101">
         <v>6</v>
       </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="101"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="B75" s="7">
+      <c r="B75" s="101">
         <v>4</v>
       </c>
     </row>
@@ -2620,7 +2636,7 @@
       <c r="C79" s="58"/>
     </row>
     <row r="80" spans="1:3" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A80" s="66" t="s">
+      <c r="A80" s="63" t="s">
         <v>89</v>
       </c>
       <c r="B80" s="41">
@@ -2635,7 +2651,7 @@
       <c r="B81" s="43">
         <v>-20</v>
       </c>
-      <c r="C81" s="67" t="s">
+      <c r="C81" s="64" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>